<commit_message>
fixed removing all values in client name (end date only) column
</commit_message>
<xml_diff>
--- a/week4/w4d1/Week_4_Cleaned.xlsx
+++ b/week4/w4d1/Week_4_Cleaned.xlsx
@@ -589,7 +589,7 @@
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,11 @@
           <t>Employed</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Alex Johnson(Wellington FL) Starts 07/14/2025 End  02/09/26</t>
+        </is>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>Supported Employment Service Only</t>
@@ -639,7 +643,7 @@
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -665,7 +669,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Taylor Smith(Sanford FL,) Lost job; needs employment </t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>ES &amp;PPT's</t>
@@ -691,7 +699,7 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -729,7 +737,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Jordan Brown(Orlando) Urgent Placement Part Time Only</t>
+        </is>
+      </c>
       <c r="M5" t="inlineStr">
         <is>
           <t>Supported Employment Service Only</t>
@@ -783,7 +795,7 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -817,7 +829,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Casey Davis(Kissimmee) Urgent Placement</t>
+        </is>
+      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>Supp ES, OJT &amp; PPT</t>
@@ -871,7 +887,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -891,7 +907,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Riley Martinez(kissimmee)-/Urgent Placement </t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -937,7 +957,7 @@
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -969,7 +989,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Morgan Lee(Casselberry FL) - Urgent Employment  interview 7/28</t>
+        </is>
+      </c>
       <c r="M8" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -1003,7 +1027,7 @@
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1053,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Avery Wilson(Winter Springs FL) Urgent Employment</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr">
         <is>
           <t>ES &amp; PPT</t>
@@ -1060,7 +1088,7 @@
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1116,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Cameron Clark( Orlando FL, ) Greeter Urgent Placement/</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr">
         <is>
           <t>Supported ES &amp; OJT</t>
@@ -1119,7 +1151,7 @@
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1177,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Jamie Lewis(Apopka FL) Urgent Placement</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr">
         <is>
           <t>Supported Employment Service Only</t>
@@ -1171,7 +1207,7 @@
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1193,7 +1229,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Peyton Hall(Orlando FL) Working on PPT completion </t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr">
         <is>
           <t>PPTs Only</t>
@@ -1219,7 +1259,7 @@
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1293,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dakota Young(Clermont) Urgent Placement </t>
+        </is>
+      </c>
       <c r="M13" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -1307,7 +1351,7 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1385,11 @@
           <t>Employed</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Skyler Allen(Maitland FL, ) Urgent placement/ Start 7/29</t>
+        </is>
+      </c>
       <c r="M14" t="inlineStr">
         <is>
           <t>ES,OJT,PPT &amp; SA</t>
@@ -1367,7 +1415,7 @@
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1409,7 +1457,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Quinn Wright(Lake Mary FL, ) Urgent placement</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -1435,7 +1487,7 @@
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1465,7 +1517,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Reese King(Lake Mary FL,) Urgent Placement</t>
+        </is>
+      </c>
       <c r="M16" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -1491,7 +1547,7 @@
       <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1593,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Harper Scott- St. Cloud, FL | Urgent Placement // waiting to receive the assessment from TJMAXX </t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr">
         <is>
           <t xml:space="preserve">Supp ES, PPT &amp; OJT </t>
@@ -1568,7 +1628,7 @@
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1592,7 +1652,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Drew Green(West Palm Beach FL) Pending job</t>
+        </is>
+      </c>
       <c r="M18" t="inlineStr">
         <is>
           <t>Supp ES &amp; PPT</t>
@@ -1622,7 +1686,7 @@
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1646,7 +1710,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Shawn Adams(Clermont FL) Urgent placement/ Interview with Frontier Airlines</t>
+        </is>
+      </c>
       <c r="M19" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -1672,7 +1740,7 @@
       <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1764,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr"/>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Kendall Nelson(Umatilla FL) Urgent placement Interview W/AmeraHealth</t>
+        </is>
+      </c>
       <c r="M20" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -1723,7 +1795,7 @@
       <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1829,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr"/>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blake Hill(Orlando FL)- (Kissimmee ONLY) </t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr">
         <is>
           <t>Supp ES, OJT &amp; PPT</t>
@@ -1791,7 +1867,7 @@
       <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1829,7 +1905,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr"/>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Emerson Baker(Sanford FL) Urgent Placement</t>
+        </is>
+      </c>
       <c r="M22" t="inlineStr">
         <is>
           <t>Supp ES, OJT &amp; PPT</t>
@@ -1855,7 +1935,7 @@
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1959,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Logan Perez-Verdejo (Kissimmee FL,)  </t>
+        </is>
+      </c>
       <c r="M23" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -1905,7 +1989,7 @@
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1929,7 +2013,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Charlie Rivera()- HE/HIM Client prefers to go by 'Bryce' (Greenacres FL,) </t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -1956,7 +2044,7 @@
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -1990,7 +2078,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr"/>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Rowan Cox-Valentin (Auburndale FL,)</t>
+        </is>
+      </c>
       <c r="M25" t="inlineStr">
         <is>
           <t>ES, OJT, PPT &amp; SA</t>
@@ -2013,7 +2105,7 @@
       <c r="W25" t="inlineStr"/>
       <c r="X25" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2039,7 +2131,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr"/>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Finley Ramirez(Winter Garden FL)</t>
+        </is>
+      </c>
       <c r="M26" t="inlineStr">
         <is>
           <t>Supported ES &amp; PPT</t>
@@ -2062,7 +2158,7 @@
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2096,7 +2192,11 @@
           <t>Employment &amp; Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr"/>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jesse Morgan(Poinciana FL)  Found a commission-based job; VRC to be contacted </t>
+        </is>
+      </c>
       <c r="M27" t="inlineStr">
         <is>
           <t>Supp ES, OJT &amp; PPT</t>
@@ -2127,7 +2227,7 @@
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2165,7 +2265,11 @@
           <t>Employment &amp; Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr"/>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Alex Johnson(Kissimmee FL) Urgent Placement Interview W applebees 8/4</t>
+        </is>
+      </c>
       <c r="M28" t="inlineStr">
         <is>
           <t>Supp ES, OJT &amp; PPT</t>
@@ -2196,7 +2300,7 @@
       <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2220,7 +2324,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Taylor Smith(Orlando FL,) Interested in House of Blends and Orlando PB </t>
+        </is>
+      </c>
       <c r="M29" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -2247,7 +2355,7 @@
       <c r="W29" t="inlineStr"/>
       <c r="X29" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2273,7 +2381,11 @@
           <t>Pending Ojt Placement</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr"/>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Jordan Brown(Orlando,FL)  Waiting for signatures to start OJT</t>
+        </is>
+      </c>
       <c r="M30" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -2299,7 +2411,7 @@
       <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2323,7 +2435,11 @@
           <t>Intake Scheduled</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr"/>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Casey Davis(Apopka FL) Intake 7/30</t>
+        </is>
+      </c>
       <c r="M31" t="inlineStr">
         <is>
           <t>YWRT &amp; SA</t>
@@ -2346,7 +2462,7 @@
       <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2370,7 +2486,11 @@
           <t>New Client - Intake Needed</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Riley Martinez(Clermont FL) </t>
+        </is>
+      </c>
       <c r="M32" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -2393,7 +2513,7 @@
       <c r="W32" t="inlineStr"/>
       <c r="X32" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2539,11 @@
           <t>Intake Scheduled</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr"/>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Morgan Lee(Winter Haven FL) intake 8/6 @1PM</t>
+        </is>
+      </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
@@ -2433,7 +2557,7 @@
       <c r="W33" t="inlineStr"/>
       <c r="X33" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2459,7 +2583,11 @@
           <t>New Client - Intake Needed</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr"/>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Avery Wilson(Lake Wales FL)</t>
+        </is>
+      </c>
       <c r="M34" t="inlineStr">
         <is>
           <t>Self-Advocacy</t>
@@ -2477,7 +2605,7 @@
       <c r="W34" t="inlineStr"/>
       <c r="X34" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2507,7 +2635,11 @@
           <t>New Client - Intake Needed</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr"/>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Cameron Clark(Sanford FL)</t>
+        </is>
+      </c>
       <c r="M35" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -2529,7 +2661,7 @@
       <c r="W35" t="inlineStr"/>
       <c r="X35" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2559,7 +2691,7 @@
       <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2593,7 +2725,7 @@
       <c r="W37" t="inlineStr"/>
       <c r="X37" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2653,7 +2785,11 @@
           <t>Client Status</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr"/>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Jamie Lewis</t>
+        </is>
+      </c>
       <c r="M38" t="inlineStr">
         <is>
           <t>Services/Referral</t>
@@ -2703,7 +2839,7 @@
       <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2723,7 +2859,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L39" t="inlineStr"/>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Peyton Hall(Winter Springs FL)   End Date 05/14/25</t>
+        </is>
+      </c>
       <c r="M39" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -2753,7 +2893,7 @@
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2913,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr"/>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Dakota Young(Orlando, FL) -  Retial Dressing Room</t>
+        </is>
+      </c>
       <c r="M40" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -2803,7 +2947,7 @@
       <c r="W40" t="inlineStr"/>
       <c r="X40" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2823,7 +2967,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr"/>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Skyler Allen(Orlando)  Dishwasher</t>
+        </is>
+      </c>
       <c r="M41" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -2853,7 +3001,7 @@
       <c r="W41" t="inlineStr"/>
       <c r="X41" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2873,7 +3021,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr"/>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Quinn Wright(Orlando, FL)  Social Service Remote</t>
+        </is>
+      </c>
       <c r="M42" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -2899,7 +3051,7 @@
       <c r="W42" t="inlineStr"/>
       <c r="X42" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2919,7 +3071,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr"/>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Reese King(Orlando FL )-Retail</t>
+        </is>
+      </c>
       <c r="M43" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -2945,7 +3101,7 @@
       <c r="W43" t="inlineStr"/>
       <c r="X43" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -2965,7 +3121,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr"/>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Harper Scott(Apopka, FL)  Dishwasher</t>
+        </is>
+      </c>
       <c r="M44" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -2987,7 +3147,7 @@
       <c r="W44" t="inlineStr"/>
       <c r="X44" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3011,7 +3171,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr"/>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Drew Green(Kissimmee, FL ) Employment Plan needed </t>
+        </is>
+      </c>
       <c r="M45" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -3037,7 +3201,7 @@
       <c r="W45" t="inlineStr"/>
       <c r="X45" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3221,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr"/>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Shawn Adams(Altamonte Springs FL) Part-Time Assembling Work</t>
+        </is>
+      </c>
       <c r="M46" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -3079,7 +3247,7 @@
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3099,7 +3267,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr"/>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Kendall Nelson(Orlando FL)</t>
+        </is>
+      </c>
       <c r="M47" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -3121,7 +3293,7 @@
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3151,7 +3323,7 @@
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3181,7 +3353,7 @@
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3215,7 +3387,7 @@
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3275,7 +3447,11 @@
           <t>Client Status</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr"/>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Blake Hill</t>
+        </is>
+      </c>
       <c r="M51" t="inlineStr">
         <is>
           <t>Services/Referral</t>
@@ -3325,7 +3501,7 @@
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3361,7 +3537,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr"/>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Emerson Baker(Mulberry-Lakleand) - Urgent Placement //applied to local restaurants</t>
+        </is>
+      </c>
       <c r="M52" t="inlineStr">
         <is>
           <t>Supported Employment Service Only</t>
@@ -3405,7 +3585,7 @@
       <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3433,7 +3613,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr"/>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Logan Perez(Lakeland FL) (stock Clerk) Urgent placement </t>
+        </is>
+      </c>
       <c r="M53" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -3471,7 +3655,7 @@
       <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3503,7 +3687,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L54" t="inlineStr"/>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Charlie Rivera(Lakeland FL) - Urgent placement // applying for bussing and hotels </t>
+        </is>
+      </c>
       <c r="M54" t="inlineStr">
         <is>
           <t>Supported Employment Service Only</t>
@@ -3545,7 +3733,7 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3569,7 +3757,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L55" t="inlineStr"/>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rowan Cox(Lake Wales FL) - Urgent placement </t>
+        </is>
+      </c>
       <c r="M55" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -3596,7 +3788,7 @@
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3620,7 +3812,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L56" t="inlineStr"/>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finley Ramirez(Winter Haven FL) Urgent placement - Famous Tate, Wlmart, WaWa near him </t>
+        </is>
+      </c>
       <c r="M56" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -3646,7 +3842,7 @@
       <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3678,7 +3874,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr"/>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jesse Morgan(Orlando)  Working on closure/transfer to new vendor </t>
+        </is>
+      </c>
       <c r="M57" t="inlineStr">
         <is>
           <t>ES &amp; PPT</t>
@@ -3708,7 +3908,7 @@
       <c r="W57" t="inlineStr"/>
       <c r="X57" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3738,7 +3938,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L58" t="inlineStr"/>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Alex Johnson(Lakeland FL,) Working on PPTs</t>
+        </is>
+      </c>
       <c r="M58" t="inlineStr">
         <is>
           <t>ES &amp; PPT</t>
@@ -3769,7 +3973,7 @@
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3801,7 +4005,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L59" t="inlineStr"/>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Taylor Smith(Lakeland, FL) - Urgent placement general maintenance</t>
+        </is>
+      </c>
       <c r="M59" t="inlineStr">
         <is>
           <t>ES, SA &amp; OJT</t>
@@ -3827,7 +4035,7 @@
       <c r="W59" t="inlineStr"/>
       <c r="X59" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3855,7 +4063,11 @@
           <t>Ojt Ended - Ready For Reimbursement</t>
         </is>
       </c>
-      <c r="L60" t="inlineStr"/>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Jordan Brown(Casselberry FL)</t>
+        </is>
+      </c>
       <c r="M60" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -3889,7 +4101,7 @@
       <c r="W60" t="inlineStr"/>
       <c r="X60" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3919,7 +4131,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr"/>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Casey Davis(Lakeland FL, ) OJT begins 07/31/2025</t>
+        </is>
+      </c>
       <c r="M61" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -3946,7 +4162,7 @@
       <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -3976,7 +4192,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr"/>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Riley Martinez(Lakeland FL) H4H ReStore in the works </t>
+        </is>
+      </c>
       <c r="M62" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -4002,7 +4222,7 @@
       <c r="W62" t="inlineStr"/>
       <c r="X62" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4032,7 +4252,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr"/>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Morgan Lee(Lakeland FL) - Equestrian centers contacted; waiting to hear back </t>
+        </is>
+      </c>
       <c r="M63" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -4058,7 +4282,7 @@
       <c r="W63" t="inlineStr"/>
       <c r="X63" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4082,7 +4306,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L64" t="inlineStr"/>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Avery Wilson(Winter Haven FL) - </t>
+        </is>
+      </c>
       <c r="M64" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -4104,7 +4332,7 @@
       <c r="W64" t="inlineStr"/>
       <c r="X64" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4140,7 +4368,11 @@
           <t>Employed</t>
         </is>
       </c>
-      <c r="L65" t="inlineStr"/>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Cameron Clark-Lavalle (Kissimmee)- VR Supervisor contacted regarding IPE change  End Date 9/17/2025</t>
+        </is>
+      </c>
       <c r="M65" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -4178,7 +4410,7 @@
       <c r="W65" t="inlineStr"/>
       <c r="X65" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4202,7 +4434,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L66" t="inlineStr"/>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jamie Lewis(Winter Haven FL, ) // VRC will be closing the case </t>
+        </is>
+      </c>
       <c r="M66" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -4228,7 +4464,7 @@
       <c r="W66" t="inlineStr"/>
       <c r="X66" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4258,7 +4494,7 @@
       <c r="W67" t="inlineStr"/>
       <c r="X67" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4288,7 +4524,7 @@
       <c r="W68" t="inlineStr"/>
       <c r="X68" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4322,7 +4558,7 @@
       <c r="W69" t="inlineStr"/>
       <c r="X69" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4382,7 +4618,11 @@
           <t>Client Status</t>
         </is>
       </c>
-      <c r="L70" t="inlineStr"/>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Peyton Hall(END DATE ONLY)</t>
+        </is>
+      </c>
       <c r="M70" t="inlineStr">
         <is>
           <t>Services/Referral</t>
@@ -4432,7 +4672,7 @@
       <c r="W70" t="inlineStr"/>
       <c r="X70" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4452,7 +4692,11 @@
           <t>Employed</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr"/>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Dakota Young(Orlando FL) 9/16/2025</t>
+        </is>
+      </c>
       <c r="M71" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -4474,7 +4718,7 @@
       <c r="W71" t="inlineStr"/>
       <c r="X71" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4498,7 +4742,11 @@
           <t>Employed</t>
         </is>
       </c>
-      <c r="L72" t="inlineStr"/>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Skyler Allen(Ocoee FL)  8/12/2025</t>
+        </is>
+      </c>
       <c r="M72" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -4524,7 +4772,7 @@
       <c r="W72" t="inlineStr"/>
       <c r="X72" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4564,7 +4812,11 @@
           <t>Employed</t>
         </is>
       </c>
-      <c r="L73" t="inlineStr"/>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Quinn Wright(Ocoee) end Date 9/28/2025</t>
+        </is>
+      </c>
       <c r="M73" t="inlineStr">
         <is>
           <t>Supp ES &amp; WBLE</t>
@@ -4610,7 +4862,7 @@
       <c r="W73" t="inlineStr"/>
       <c r="X73" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4640,7 +4892,11 @@
           <t>Employed</t>
         </is>
       </c>
-      <c r="L74" t="inlineStr"/>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Reese King(WEST PALM BEACH FL) End date 09/29/25</t>
+        </is>
+      </c>
       <c r="M74" t="inlineStr">
         <is>
           <t>Supp ES &amp; PPT</t>
@@ -4667,7 +4923,7 @@
       <c r="W74" t="inlineStr"/>
       <c r="X74" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4703,7 +4959,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L75" t="inlineStr"/>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Harper Scott(Ocoee FL)-  8/9/2025</t>
+        </is>
+      </c>
       <c r="M75" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -4745,7 +5005,7 @@
       <c r="W75" t="inlineStr"/>
       <c r="X75" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4783,7 +5043,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L76" t="inlineStr"/>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Drew Green(Geneva FL,) 8/13/2025</t>
+        </is>
+      </c>
       <c r="M76" t="inlineStr">
         <is>
           <t xml:space="preserve">Supp ES, PPT &amp; OJT </t>
@@ -4809,7 +5073,7 @@
       <c r="W76" t="inlineStr"/>
       <c r="X76" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4847,7 +5111,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L77" t="inlineStr"/>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Shawn Adams(Lake Mary FL)  end date:9/24/2025</t>
+        </is>
+      </c>
       <c r="M77" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -4878,7 +5146,7 @@
       <c r="W77" t="inlineStr"/>
       <c r="X77" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4912,7 +5180,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L78" t="inlineStr"/>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Kendall Nelson(Apopka FL)-END DATE 9/25</t>
+        </is>
+      </c>
       <c r="M78" t="inlineStr">
         <is>
           <t>WBLE &amp; YWRT</t>
@@ -4930,7 +5202,7 @@
       <c r="W78" t="inlineStr"/>
       <c r="X78" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -4964,7 +5236,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L79" t="inlineStr"/>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Blake Hill(DELTONA FL)  END DATE 9/25</t>
+        </is>
+      </c>
       <c r="M79" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -4990,7 +5266,7 @@
       <c r="W79" t="inlineStr"/>
       <c r="X79" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5022,7 +5298,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L80" t="inlineStr"/>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Emerson Baker(Orlando FL, ) END DATE 9/27/2025</t>
+        </is>
+      </c>
       <c r="M80" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5048,7 +5328,7 @@
       <c r="W80" t="inlineStr"/>
       <c r="X80" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5074,7 +5354,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L81" t="inlineStr"/>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Logan Perez(Windermere FL) end date:9/25/2025</t>
+        </is>
+      </c>
       <c r="M81" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -5101,7 +5385,7 @@
       <c r="W81" t="inlineStr"/>
       <c r="X81" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5417,11 @@
           <t>Pending Ojt</t>
         </is>
       </c>
-      <c r="L82" t="inlineStr"/>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Charlie Rivera(Orlando FL) (21 y/o) Share the care Meet &amp; Greet 8/5</t>
+        </is>
+      </c>
       <c r="M82" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -5155,7 +5443,7 @@
       <c r="W82" t="inlineStr"/>
       <c r="X82" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5179,7 +5467,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L83" t="inlineStr"/>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Rowan Cox(Orlando FL)  10/01/25</t>
+        </is>
+      </c>
       <c r="M83" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -5206,7 +5498,7 @@
       <c r="W83" t="inlineStr"/>
       <c r="X83" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5238,7 +5530,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr"/>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finley Ramirez-Matos (KISSIMMEE FL) (18 y/o) Cafe? </t>
+        </is>
+      </c>
       <c r="M84" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -5260,7 +5556,7 @@
       <c r="W84" t="inlineStr"/>
       <c r="X84" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5292,7 +5588,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr"/>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Jesse Morgan(Ocoee FL,)House of Blends? Parent would like to wait for school to start and his schedule is established.</t>
+        </is>
+      </c>
       <c r="M85" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5310,7 +5610,7 @@
       <c r="W85" t="inlineStr"/>
       <c r="X85" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5342,7 +5642,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr"/>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Alex Johnson(Ocoee FL) (walker; 15y/o) House of Blends?</t>
+        </is>
+      </c>
       <c r="M86" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5360,7 +5664,7 @@
       <c r="W86" t="inlineStr"/>
       <c r="X86" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5392,7 +5696,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L87" t="inlineStr"/>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Taylor Smith(Orlando FL) Aloma Cinema Grill?</t>
+        </is>
+      </c>
       <c r="M87" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5410,7 +5718,7 @@
       <c r="W87" t="inlineStr"/>
       <c r="X87" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5442,7 +5750,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L88" t="inlineStr"/>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Jordan Brown(Orlando FL) Aloma Cinema Grill?</t>
+        </is>
+      </c>
       <c r="M88" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5460,7 +5772,7 @@
       <c r="W88" t="inlineStr"/>
       <c r="X88" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5492,7 +5804,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L89" t="inlineStr"/>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Casey Davis(Orlando FL) (18 y/o) </t>
+        </is>
+      </c>
       <c r="M89" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5510,7 +5826,7 @@
       <c r="W89" t="inlineStr"/>
       <c r="X89" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5542,7 +5858,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L90" t="inlineStr"/>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Riley Martinez-Gonzalez (KISSIMMEE FL) (17 y/o)</t>
+        </is>
+      </c>
       <c r="M90" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5560,7 +5880,7 @@
       <c r="W90" t="inlineStr"/>
       <c r="X90" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5596,7 +5916,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L91" t="inlineStr"/>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Morgan Lee(Orlando FL) (17 y/o) </t>
+        </is>
+      </c>
       <c r="M91" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5623,7 +5947,7 @@
       <c r="W91" t="inlineStr"/>
       <c r="X91" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5647,7 +5971,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L92" t="inlineStr"/>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Avery Wilson(Orlando FL,) </t>
+        </is>
+      </c>
       <c r="M92" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -5670,7 +5998,7 @@
       <c r="W92" t="inlineStr"/>
       <c r="X92" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5700,7 +6028,11 @@
           <t>New Client - Intake Needed</t>
         </is>
       </c>
-      <c r="L93" t="inlineStr"/>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>Cameron Clark(Saint Cloud FL) Pending - A Place for Grace intake 7/31</t>
+        </is>
+      </c>
       <c r="M93" t="inlineStr">
         <is>
           <t>YWRT, WBLE &amp; SA</t>
@@ -5718,7 +6050,7 @@
       <c r="W93" t="inlineStr"/>
       <c r="X93" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5748,7 +6080,7 @@
       <c r="W94" t="inlineStr"/>
       <c r="X94" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5778,7 +6110,7 @@
       <c r="W95" t="inlineStr"/>
       <c r="X95" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5808,7 +6140,7 @@
       <c r="W96" t="inlineStr"/>
       <c r="X96" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5838,7 +6170,7 @@
       <c r="W97" t="inlineStr"/>
       <c r="X97" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5868,7 +6200,7 @@
       <c r="W98" t="inlineStr"/>
       <c r="X98" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5902,7 +6234,7 @@
       <c r="W99" t="inlineStr"/>
       <c r="X99" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -5962,7 +6294,11 @@
           <t>Client Status</t>
         </is>
       </c>
-      <c r="L100" t="inlineStr"/>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>Jamie Lewis(END DATE ONLY)</t>
+        </is>
+      </c>
       <c r="M100" t="inlineStr">
         <is>
           <t>Services/Referral</t>
@@ -6012,7 +6348,7 @@
       <c r="W100" t="inlineStr"/>
       <c r="X100" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6040,7 +6376,11 @@
           <t>On Pause</t>
         </is>
       </c>
-      <c r="L101" t="inlineStr"/>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Peyton Hall(Kissimmee FL)-Due to Anxiety/Panic Attacks </t>
+        </is>
+      </c>
       <c r="M101" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -6070,7 +6410,7 @@
       <c r="W101" t="inlineStr"/>
       <c r="X101" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6098,7 +6438,11 @@
           <t>On Pause</t>
         </is>
       </c>
-      <c r="L102" t="inlineStr"/>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>Dakota Young(Cloud FL)  (Grandmom stated that he is in the hospital)</t>
+        </is>
+      </c>
       <c r="M102" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -6121,7 +6465,7 @@
       <c r="W102" t="inlineStr"/>
       <c r="X102" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6145,7 +6489,11 @@
           <t>On Pause</t>
         </is>
       </c>
-      <c r="L103" t="inlineStr"/>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>Skyler Allen(Sanford)-On Pause 6 mo/Health Issues</t>
+        </is>
+      </c>
       <c r="M103" t="inlineStr"/>
       <c r="N103" t="inlineStr">
         <is>
@@ -6171,7 +6519,7 @@
       <c r="W103" t="inlineStr"/>
       <c r="X103" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6195,7 +6543,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L104" t="inlineStr"/>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>Quinn Wright(WEST PALM BEACH FL)= currently working at temp agency/ On Pause-out of Town VRC unsure if he is returning</t>
+        </is>
+      </c>
       <c r="M104" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -6225,7 +6577,7 @@
       <c r="W104" t="inlineStr"/>
       <c r="X104" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6251,7 +6603,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L105" t="inlineStr"/>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reese King(WPB) (Blind/Creole) </t>
+        </is>
+      </c>
       <c r="M105" t="inlineStr">
         <is>
           <t>Supp ES &amp; PPT</t>
@@ -6281,7 +6637,7 @@
       <c r="W105" t="inlineStr"/>
       <c r="X105" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6315,7 +6671,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L106" t="inlineStr"/>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Harper Scott(Winter Springs) end date: 07/06/25 site visit every week </t>
+        </is>
+      </c>
       <c r="M106" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -6341,7 +6701,7 @@
       <c r="W106" t="inlineStr"/>
       <c r="X106" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6361,7 +6721,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L107" t="inlineStr"/>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>Drew Green(Orlando FL)  End Date  05/19/25</t>
+        </is>
+      </c>
       <c r="M107" t="inlineStr">
         <is>
           <t>Supported Employment Service Only</t>
@@ -6391,7 +6755,7 @@
       <c r="W107" t="inlineStr"/>
       <c r="X107" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6423,7 +6787,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L108" t="inlineStr"/>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>Shawn Adams(Orlando FL) Contact issues since started program</t>
+        </is>
+      </c>
       <c r="M108" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -6446,7 +6814,7 @@
       <c r="W108" t="inlineStr"/>
       <c r="X108" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6472,7 +6840,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L109" t="inlineStr"/>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kendall Nelson(Groveland FL,) Pending Closure </t>
+        </is>
+      </c>
       <c r="M109" t="inlineStr">
         <is>
           <t>Supported ES &amp; PPT</t>
@@ -6499,7 +6871,7 @@
       <c r="W109" t="inlineStr"/>
       <c r="X109" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6533,7 +6905,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L110" t="inlineStr"/>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blake Hill(Davenport FL) ES-RD </t>
+        </is>
+      </c>
       <c r="M110" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -6556,7 +6932,7 @@
       <c r="W110" t="inlineStr"/>
       <c r="X110" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6586,7 +6962,7 @@
       <c r="W111" t="inlineStr"/>
       <c r="X111" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6614,7 +6990,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L112" t="inlineStr"/>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emerson Baker(Orlando FL)-end date 02/18/25 </t>
+        </is>
+      </c>
       <c r="M112" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -6660,7 +7040,7 @@
       </c>
       <c r="X112" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6688,7 +7068,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L113" t="inlineStr"/>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>Logan Perez(Orlando FL) Client needs all day supervision</t>
+        </is>
+      </c>
       <c r="M113" t="inlineStr">
         <is>
           <t>Supported ES &amp; OJT</t>
@@ -6711,7 +7095,7 @@
       <c r="W113" t="inlineStr"/>
       <c r="X113" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6737,7 +7121,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L114" t="inlineStr"/>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>Charlie Rivera(WPB)-Wheelchair (12) End Date(11/18/2024)</t>
+        </is>
+      </c>
       <c r="M114" t="inlineStr">
         <is>
           <t>ES with PPTs</t>
@@ -6791,7 +7179,7 @@
       </c>
       <c r="X114" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6819,7 +7207,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L115" t="inlineStr"/>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>Rowan Cox(Orlando FL)   (11/12/24)</t>
+        </is>
+      </c>
       <c r="M115" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -6849,7 +7241,7 @@
       <c r="W115" t="inlineStr"/>
       <c r="X115" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6873,7 +7265,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L116" t="inlineStr"/>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>Finley Ramirez( Orlando) (11/11/24)</t>
+        </is>
+      </c>
       <c r="M116" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -6919,7 +7315,7 @@
       <c r="W116" t="inlineStr"/>
       <c r="X116" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -6953,7 +7349,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L117" t="inlineStr"/>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jesse Morgan(Sanford FL,) (Janitor) </t>
+        </is>
+      </c>
       <c r="M117" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -6987,7 +7387,7 @@
       <c r="W117" t="inlineStr"/>
       <c r="X117" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7011,7 +7411,11 @@
           <t>Contact Issues</t>
         </is>
       </c>
-      <c r="L118" t="inlineStr"/>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>Alex Johnson(West Palm Beach FL)</t>
+        </is>
+      </c>
       <c r="M118" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -7053,7 +7457,7 @@
       <c r="W118" t="inlineStr"/>
       <c r="X118" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7089,7 +7493,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L119" t="inlineStr"/>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>Taylor Smith(Fairview Shores) (15) (3/4/2024)</t>
+        </is>
+      </c>
       <c r="M119" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -7127,7 +7535,7 @@
       <c r="W119" t="inlineStr"/>
       <c r="X119" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7151,7 +7559,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L120" t="inlineStr"/>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>Jordan Brown(Orlando) (19) (3/7/2024)</t>
+        </is>
+      </c>
       <c r="M120" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -7189,7 +7601,7 @@
       <c r="W120" t="inlineStr"/>
       <c r="X120" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7213,7 +7625,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L121" t="inlineStr"/>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>Casey Davis(Apopka)(5/24/2024)</t>
+        </is>
+      </c>
       <c r="M121" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -7259,7 +7675,7 @@
       </c>
       <c r="X121" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7287,7 +7703,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L122" t="inlineStr"/>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>Riley Martinez(Orlando) (25)(2/8/24)</t>
+        </is>
+      </c>
       <c r="M122" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -7321,7 +7741,7 @@
       <c r="W122" t="inlineStr"/>
       <c r="X122" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7349,7 +7769,11 @@
           <t>On Pause</t>
         </is>
       </c>
-      <c r="L123" t="inlineStr"/>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Morgan Lee(Orlando) </t>
+        </is>
+      </c>
       <c r="M123" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -7383,7 +7807,7 @@
       <c r="W123" t="inlineStr"/>
       <c r="X123" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7441,7 +7865,7 @@
       <c r="W124" t="inlineStr"/>
       <c r="X124" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7475,7 +7899,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L125" t="inlineStr"/>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Avery Wilson-Colon, Sol Luis (Orlando) *Meeting w/VRC </t>
+        </is>
+      </c>
       <c r="M125" t="inlineStr">
         <is>
           <t>Supp ES, OJT &amp; PPT</t>
@@ -7505,7 +7933,7 @@
       <c r="W125" t="inlineStr"/>
       <c r="X125" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7533,7 +7961,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L126" t="inlineStr"/>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>Cameron Clark(Kissimmee) (19) * Meeting w/ VRC</t>
+        </is>
+      </c>
       <c r="M126" t="inlineStr">
         <is>
           <t>Supported ES &amp; OJT</t>
@@ -7567,7 +7999,7 @@
       <c r="W126" t="inlineStr"/>
       <c r="X126" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7587,7 +8019,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L127" t="inlineStr"/>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>Jamie Lewis</t>
+        </is>
+      </c>
       <c r="M127" t="inlineStr">
         <is>
           <t>ES with PPTs</t>
@@ -7605,7 +8041,7 @@
       <c r="W127" t="inlineStr"/>
       <c r="X127" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7625,7 +8061,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L128" t="inlineStr"/>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>Peyton Hall</t>
+        </is>
+      </c>
       <c r="M128" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -7647,7 +8087,7 @@
       <c r="W128" t="inlineStr"/>
       <c r="X128" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7667,7 +8107,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L129" t="inlineStr"/>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>Dakota Young</t>
+        </is>
+      </c>
       <c r="M129" t="inlineStr"/>
       <c r="N129" t="inlineStr"/>
       <c r="O129" t="inlineStr"/>
@@ -7681,7 +8125,7 @@
       <c r="W129" t="inlineStr"/>
       <c r="X129" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7701,7 +8145,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L130" t="inlineStr"/>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>Skyler Allen</t>
+        </is>
+      </c>
       <c r="M130" t="inlineStr"/>
       <c r="N130" t="inlineStr"/>
       <c r="O130" t="inlineStr"/>
@@ -7715,7 +8163,7 @@
       <c r="W130" t="inlineStr"/>
       <c r="X130" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7735,7 +8183,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L131" t="inlineStr"/>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>Quinn Wright</t>
+        </is>
+      </c>
       <c r="M131" t="inlineStr"/>
       <c r="N131" t="inlineStr"/>
       <c r="O131" s="2" t="n">
@@ -7751,7 +8203,7 @@
       <c r="W131" t="inlineStr"/>
       <c r="X131" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7783,7 +8235,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L132" t="inlineStr"/>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reese King(WPB) (7) </t>
+        </is>
+      </c>
       <c r="M132" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -7805,7 +8261,7 @@
       <c r="W132" t="inlineStr"/>
       <c r="X132" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7835,7 +8291,7 @@
       <c r="W133" t="inlineStr"/>
       <c r="X133" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7869,7 +8325,7 @@
       <c r="W134" t="inlineStr"/>
       <c r="X134" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7899,7 +8355,7 @@
       <c r="W135" t="inlineStr"/>
       <c r="X135" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7929,7 +8385,7 @@
       <c r="W136" t="inlineStr"/>
       <c r="X136" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7963,7 +8419,7 @@
       <c r="W137" t="inlineStr"/>
       <c r="X137" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -7993,7 +8449,7 @@
       <c r="W138" t="inlineStr"/>
       <c r="X138" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8023,7 +8479,7 @@
       <c r="W139" t="inlineStr"/>
       <c r="X139" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8057,7 +8513,7 @@
       <c r="W140" t="inlineStr"/>
       <c r="X140" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8087,7 +8543,7 @@
       <c r="W141" t="inlineStr"/>
       <c r="X141" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8117,7 +8573,7 @@
       <c r="W142" t="inlineStr"/>
       <c r="X142" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8147,7 +8603,7 @@
       <c r="W143" t="inlineStr"/>
       <c r="X143" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8177,7 +8633,7 @@
       <c r="W144" t="inlineStr"/>
       <c r="X144" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8211,7 +8667,7 @@
       <c r="W145" t="inlineStr"/>
       <c r="X145" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8241,7 +8697,7 @@
       <c r="W146" t="inlineStr"/>
       <c r="X146" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8271,7 +8727,7 @@
       <c r="W147" t="inlineStr"/>
       <c r="X147" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8301,7 +8757,7 @@
       <c r="W148" t="inlineStr"/>
       <c r="X148" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8331,7 +8787,7 @@
       <c r="W149" t="inlineStr"/>
       <c r="X149" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8361,7 +8817,7 @@
       <c r="W150" t="inlineStr"/>
       <c r="X150" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8391,7 +8847,7 @@
       <c r="W151" t="inlineStr"/>
       <c r="X151" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8421,7 +8877,7 @@
       <c r="W152" t="inlineStr"/>
       <c r="X152" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8451,7 +8907,7 @@
       <c r="W153" t="inlineStr"/>
       <c r="X153" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8481,7 +8937,7 @@
       <c r="W154" t="inlineStr"/>
       <c r="X154" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8511,7 +8967,7 @@
       <c r="W155" t="inlineStr"/>
       <c r="X155" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8541,7 +8997,7 @@
       <c r="W156" t="inlineStr"/>
       <c r="X156" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8571,7 +9027,7 @@
       <c r="W157" t="inlineStr"/>
       <c r="X157" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8601,7 +9057,7 @@
       <c r="W158" t="inlineStr"/>
       <c r="X158" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8631,7 +9087,7 @@
       <c r="W159" t="inlineStr"/>
       <c r="X159" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8661,7 +9117,7 @@
       <c r="W160" t="inlineStr"/>
       <c r="X160" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8691,7 +9147,7 @@
       <c r="W161" t="inlineStr"/>
       <c r="X161" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8721,7 +9177,7 @@
       <c r="W162" t="inlineStr"/>
       <c r="X162" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8751,7 +9207,7 @@
       <c r="W163" t="inlineStr"/>
       <c r="X163" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8781,7 +9237,7 @@
       <c r="W164" t="inlineStr"/>
       <c r="X164" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8811,7 +9267,7 @@
       <c r="W165" t="inlineStr"/>
       <c r="X165" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8841,7 +9297,7 @@
       <c r="W166" t="inlineStr"/>
       <c r="X166" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8871,7 +9327,7 @@
       <c r="W167" t="inlineStr"/>
       <c r="X167" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8901,7 +9357,7 @@
       <c r="W168" t="inlineStr"/>
       <c r="X168" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8931,7 +9387,7 @@
       <c r="W169" t="inlineStr"/>
       <c r="X169" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8961,7 +9417,7 @@
       <c r="W170" t="inlineStr"/>
       <c r="X170" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -8991,7 +9447,7 @@
       <c r="W171" t="inlineStr"/>
       <c r="X171" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9021,7 +9477,7 @@
       <c r="W172" t="inlineStr"/>
       <c r="X172" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9051,7 +9507,7 @@
       <c r="W173" t="inlineStr"/>
       <c r="X173" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9081,7 +9537,7 @@
       <c r="W174" t="inlineStr"/>
       <c r="X174" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9111,7 +9567,7 @@
       <c r="W175" t="inlineStr"/>
       <c r="X175" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9141,7 +9597,7 @@
       <c r="W176" t="inlineStr"/>
       <c r="X176" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9171,7 +9627,7 @@
       <c r="W177" t="inlineStr"/>
       <c r="X177" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9201,7 +9657,7 @@
       <c r="W178" t="inlineStr"/>
       <c r="X178" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9231,7 +9687,7 @@
       <c r="W179" t="inlineStr"/>
       <c r="X179" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9261,7 +9717,7 @@
       <c r="W180" t="inlineStr"/>
       <c r="X180" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9291,7 +9747,7 @@
       <c r="W181" t="inlineStr"/>
       <c r="X181" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9321,7 +9777,7 @@
       <c r="W182" t="inlineStr"/>
       <c r="X182" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9351,7 +9807,7 @@
       <c r="W183" t="inlineStr"/>
       <c r="X183" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9381,7 +9837,7 @@
       <c r="W184" t="inlineStr"/>
       <c r="X184" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9401,7 +9857,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L185" t="inlineStr"/>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>Harper Scott</t>
+        </is>
+      </c>
       <c r="M185" t="inlineStr">
         <is>
           <t>ES with PPTs</t>
@@ -9419,7 +9879,7 @@
       <c r="W185" t="inlineStr"/>
       <c r="X185" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9439,7 +9899,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L186" t="inlineStr"/>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>Drew Green</t>
+        </is>
+      </c>
       <c r="M186" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -9457,7 +9921,7 @@
       <c r="W186" t="inlineStr"/>
       <c r="X186" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9477,7 +9941,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L187" t="inlineStr"/>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>Shawn Adams</t>
+        </is>
+      </c>
       <c r="M187" t="inlineStr"/>
       <c r="N187" t="inlineStr"/>
       <c r="O187" t="inlineStr"/>
@@ -9491,7 +9959,7 @@
       <c r="W187" t="inlineStr"/>
       <c r="X187" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9511,7 +9979,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L188" t="inlineStr"/>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>Kendall Nelson</t>
+        </is>
+      </c>
       <c r="M188" t="inlineStr"/>
       <c r="N188" t="inlineStr"/>
       <c r="O188" t="inlineStr"/>
@@ -9525,7 +9997,7 @@
       <c r="W188" t="inlineStr"/>
       <c r="X188" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9545,7 +10017,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L189" t="inlineStr"/>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>Blake Hill</t>
+        </is>
+      </c>
       <c r="M189" t="inlineStr"/>
       <c r="N189" t="inlineStr"/>
       <c r="O189" t="inlineStr"/>
@@ -9559,7 +10035,7 @@
       <c r="W189" t="inlineStr"/>
       <c r="X189" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9587,7 +10063,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L190" t="inlineStr"/>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>Emerson Baker-Cue (Y)</t>
+        </is>
+      </c>
       <c r="M190" t="inlineStr">
         <is>
           <t>WBLE &amp; YWRT</t>
@@ -9605,7 +10085,7 @@
       <c r="W190" t="inlineStr"/>
       <c r="X190" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9633,7 +10113,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L191" t="inlineStr"/>
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>Logan Perez(Orlando)  (1/1/2024)</t>
+        </is>
+      </c>
       <c r="M191" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -9659,7 +10143,7 @@
       <c r="W191" t="inlineStr"/>
       <c r="X191" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9695,7 +10179,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L192" t="inlineStr"/>
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>Charlie Rivera(Orlando) (2)</t>
+        </is>
+      </c>
       <c r="M192" t="inlineStr">
         <is>
           <t>OJT &amp; PPT</t>
@@ -9733,7 +10221,7 @@
       <c r="W192" t="inlineStr"/>
       <c r="X192" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9767,7 +10255,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L193" t="inlineStr"/>
+      <c r="L193" t="inlineStr">
+        <is>
+          <t>Rowan Cox(Orlando) (16)(1/19/2024)</t>
+        </is>
+      </c>
       <c r="M193" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -9801,7 +10293,7 @@
       <c r="W193" t="inlineStr"/>
       <c r="X193" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9833,7 +10325,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L194" t="inlineStr"/>
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>Finley Ramirez(St. Cloud) (22) 03/07/2024</t>
+        </is>
+      </c>
       <c r="M194" t="inlineStr">
         <is>
           <t>Supported ES &amp; OJT</t>
@@ -9871,7 +10367,7 @@
       <c r="W194" t="inlineStr"/>
       <c r="X194" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9899,7 +10395,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L195" t="inlineStr"/>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>Jesse Morgan(Ocoee) - (26) 03/16/2024</t>
+        </is>
+      </c>
       <c r="M195" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -9937,7 +10437,7 @@
       <c r="W195" t="inlineStr"/>
       <c r="X195" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -9957,7 +10457,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L196" t="inlineStr"/>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>Alex Johnson(WPB) (12) (5/6/2024)</t>
+        </is>
+      </c>
       <c r="M196" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -9999,7 +10503,7 @@
       <c r="W196" t="inlineStr"/>
       <c r="X196" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10023,7 +10527,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L197" t="inlineStr"/>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>Taylor Smith(Winter Garden) (13) (4/16/2024)</t>
+        </is>
+      </c>
       <c r="M197" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -10065,7 +10573,7 @@
       <c r="W197" t="inlineStr"/>
       <c r="X197" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10089,7 +10597,11 @@
           <t>Services Completed</t>
         </is>
       </c>
-      <c r="L198" t="inlineStr"/>
+      <c r="L198" t="inlineStr">
+        <is>
+          <t>Jordan Brown(Lake Nona) (10)  (6/17/2024</t>
+        </is>
+      </c>
       <c r="M198" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -10139,7 +10651,7 @@
       </c>
       <c r="X198" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10167,7 +10679,11 @@
           <t>Ojt Ended - Ready For Reimbursement</t>
         </is>
       </c>
-      <c r="L199" t="inlineStr"/>
+      <c r="L199" t="inlineStr">
+        <is>
+          <t>Casey Davis(Ocoee) - (26) (7/6/24)</t>
+        </is>
+      </c>
       <c r="M199" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -10209,7 +10725,7 @@
       <c r="W199" t="inlineStr"/>
       <c r="X199" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10243,7 +10759,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L200" t="inlineStr"/>
+      <c r="L200" t="inlineStr">
+        <is>
+          <t>Riley Martinez(Orlando) (14) (7/19/2024)</t>
+        </is>
+      </c>
       <c r="M200" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -10293,7 +10813,7 @@
       </c>
       <c r="X200" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10317,7 +10837,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L201" t="inlineStr"/>
+      <c r="L201" t="inlineStr">
+        <is>
+          <t>Morgan Lee(Orlando FL) (2) (7/31/2024)</t>
+        </is>
+      </c>
       <c r="M201" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -10367,7 +10891,7 @@
       </c>
       <c r="X201" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10395,7 +10919,11 @@
           <t>Ojt Placement Needed</t>
         </is>
       </c>
-      <c r="L202" t="inlineStr"/>
+      <c r="L202" t="inlineStr">
+        <is>
+          <t>Avery Wilson(orlando)</t>
+        </is>
+      </c>
       <c r="M202" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -10417,7 +10945,7 @@
       <c r="W202" t="inlineStr"/>
       <c r="X202" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10441,7 +10969,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L203" t="inlineStr"/>
+      <c r="L203" t="inlineStr">
+        <is>
+          <t>Cameron Clark(WPB) (13)</t>
+        </is>
+      </c>
       <c r="M203" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -10479,7 +11011,7 @@
       <c r="W203" t="inlineStr"/>
       <c r="X203" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10503,7 +11035,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L204" t="inlineStr"/>
+      <c r="L204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jamie Lewis(Clermont FL) </t>
+        </is>
+      </c>
       <c r="M204" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -10553,7 +11089,7 @@
       </c>
       <c r="X204" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10581,7 +11117,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L205" t="inlineStr"/>
+      <c r="L205" t="inlineStr">
+        <is>
+          <t>Peyton Hall( DAVENPORT FL) ( Hands of Hope , Well Thifth Store)</t>
+        </is>
+      </c>
       <c r="M205" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -10603,7 +11143,7 @@
       <c r="W205" t="inlineStr"/>
       <c r="X205" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10631,7 +11171,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L206" t="inlineStr"/>
+      <c r="L206" t="inlineStr">
+        <is>
+          <t>Dakota Young(Sanford FL)</t>
+        </is>
+      </c>
       <c r="M206" t="inlineStr">
         <is>
           <t>Supported ES &amp; OJT</t>
@@ -10654,7 +11198,7 @@
       <c r="W206" t="inlineStr"/>
       <c r="X206" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10678,7 +11222,11 @@
           <t>Employment Placement Needed</t>
         </is>
       </c>
-      <c r="L207" t="inlineStr"/>
+      <c r="L207" t="inlineStr">
+        <is>
+          <t>Skyler Allen(Clermont FL)</t>
+        </is>
+      </c>
       <c r="M207" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -10708,7 +11256,7 @@
       <c r="W207" t="inlineStr"/>
       <c r="X207" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10736,7 +11284,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L208" t="inlineStr"/>
+      <c r="L208" t="inlineStr">
+        <is>
+          <t>Quinn Wright(Orlando) (18) 9/25/2024</t>
+        </is>
+      </c>
       <c r="M208" t="inlineStr">
         <is>
           <t>Supported Employment Service Only</t>
@@ -10786,7 +11338,7 @@
       </c>
       <c r="X208" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10816,7 +11368,11 @@
           <t>Ojt In Progress</t>
         </is>
       </c>
-      <c r="L209" t="inlineStr"/>
+      <c r="L209" t="inlineStr">
+        <is>
+          <t>Reese King(Casselberry FL) -10/14/24</t>
+        </is>
+      </c>
       <c r="M209" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -10850,7 +11406,7 @@
       <c r="W209" t="inlineStr"/>
       <c r="X209" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10878,7 +11434,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L210" t="inlineStr"/>
+      <c r="L210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Harper Scott(Orlando) </t>
+        </is>
+      </c>
       <c r="M210" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -10932,7 +11492,7 @@
       </c>
       <c r="X210" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -10962,7 +11522,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L211" t="inlineStr"/>
+      <c r="L211" t="inlineStr">
+        <is>
+          <t>Drew Green(Orlando) (Transportation Attendants)</t>
+        </is>
+      </c>
       <c r="M211" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -11000,7 +11564,7 @@
       <c r="W211" t="inlineStr"/>
       <c r="X211" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11038,7 +11602,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L212" t="inlineStr"/>
+      <c r="L212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shawn Adams(Lakeland) </t>
+        </is>
+      </c>
       <c r="M212" t="inlineStr">
         <is>
           <t>Supp ES, OJT &amp; PPT</t>
@@ -11092,7 +11660,7 @@
       </c>
       <c r="X212" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11122,7 +11690,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L213" t="inlineStr"/>
+      <c r="L213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kendall Nelson(Woodfield Drive Sanford)-Visual Impairment </t>
+        </is>
+      </c>
       <c r="M213" t="inlineStr">
         <is>
           <t>ES &amp;PPT's</t>
@@ -11176,7 +11748,7 @@
       </c>
       <c r="X213" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11204,7 +11776,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L214" t="inlineStr"/>
+      <c r="L214" t="inlineStr">
+        <is>
+          <t>Blake Hill(Orlando FL)- Possible Closure to APD</t>
+        </is>
+      </c>
       <c r="M214" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -11234,7 +11810,7 @@
       <c r="W214" t="inlineStr"/>
       <c r="X214" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11262,7 +11838,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L215" t="inlineStr"/>
+      <c r="L215" t="inlineStr">
+        <is>
+          <t>Emerson Baker(Orlando FL)-Possible Closure to APD</t>
+        </is>
+      </c>
       <c r="M215" t="inlineStr">
         <is>
           <t>WBLE Only</t>
@@ -11293,7 +11873,7 @@
       <c r="W215" t="inlineStr"/>
       <c r="X215" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11317,7 +11897,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L216" t="inlineStr"/>
+      <c r="L216" t="inlineStr">
+        <is>
+          <t>Logan Perez(Clermont) (10) 10/29/2024)</t>
+        </is>
+      </c>
       <c r="M216" t="inlineStr">
         <is>
           <t>Supported Employment Service Only</t>
@@ -11367,7 +11951,7 @@
       </c>
       <c r="X216" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11391,7 +11975,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L217" t="inlineStr"/>
+      <c r="L217" t="inlineStr">
+        <is>
+          <t>Charlie Rivera(WPB) End Sate 11/26/24</t>
+        </is>
+      </c>
       <c r="M217" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -11422,7 +12010,7 @@
       <c r="W217" t="inlineStr"/>
       <c r="X217" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11450,7 +12038,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L218" t="inlineStr"/>
+      <c r="L218" t="inlineStr">
+        <is>
+          <t>Rowan Cox(Davenport FL)  11/23/2024</t>
+        </is>
+      </c>
       <c r="M218" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -11504,7 +12096,7 @@
       </c>
       <c r="X218" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11532,7 +12124,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L219" t="inlineStr"/>
+      <c r="L219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finley Ramirez( Davenport FL,)-Send Email for closure </t>
+        </is>
+      </c>
       <c r="M219" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -11578,7 +12174,7 @@
       </c>
       <c r="X219" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11608,7 +12204,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L220" t="inlineStr"/>
+      <c r="L220" t="inlineStr">
+        <is>
+          <t>Jesse Morgan(Winter Springs FL)-VR needs to meet w/ her.</t>
+        </is>
+      </c>
       <c r="M220" t="inlineStr">
         <is>
           <t>Supported ES &amp; PPT</t>
@@ -11643,7 +12243,7 @@
       <c r="W220" t="inlineStr"/>
       <c r="X220" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11673,7 +12273,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L221" t="inlineStr"/>
+      <c r="L221" t="inlineStr">
+        <is>
+          <t>Alex Johnson(Orlando) (12/25/24)</t>
+        </is>
+      </c>
       <c r="M221" t="inlineStr">
         <is>
           <t>ES, OJT &amp; PPT</t>
@@ -11723,7 +12327,7 @@
       <c r="W221" t="inlineStr"/>
       <c r="X221" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11749,7 +12353,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L222" t="inlineStr"/>
+      <c r="L222" t="inlineStr">
+        <is>
+          <t>Taylor Smith(Rivera Beach) (01/03/25)</t>
+        </is>
+      </c>
       <c r="M222" t="inlineStr">
         <is>
           <t>ES &amp; PPT</t>
@@ -11803,7 +12411,7 @@
       </c>
       <c r="X222" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11831,7 +12439,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L223" t="inlineStr"/>
+      <c r="L223" t="inlineStr">
+        <is>
+          <t>Jordan Brown(Orlando) (12/27/2024)</t>
+        </is>
+      </c>
       <c r="M223" t="inlineStr">
         <is>
           <t>ES &amp; OJT</t>
@@ -11885,7 +12497,7 @@
       </c>
       <c r="X223" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Duplicate; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11913,7 +12525,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L224" t="inlineStr"/>
+      <c r="L224" t="inlineStr">
+        <is>
+          <t>Casey Davis(Davenport FL) - w/ a different provider</t>
+        </is>
+      </c>
       <c r="M224" t="inlineStr">
         <is>
           <t>OJT Only</t>
@@ -11935,7 +12551,7 @@
       <c r="W224" t="inlineStr"/>
       <c r="X224" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -11965,7 +12581,11 @@
           <t>Service(S) Completed</t>
         </is>
       </c>
-      <c r="L225" t="inlineStr"/>
+      <c r="L225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Riley Martinez(Orlando FL,) SA complete/ currently in job program O.C. </t>
+        </is>
+      </c>
       <c r="M225" t="inlineStr">
         <is>
           <t>SA &amp; WBLE</t>
@@ -11995,7 +12615,7 @@
       <c r="W225" t="inlineStr"/>
       <c r="X225" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -12021,7 +12641,11 @@
           <t>Closure Request</t>
         </is>
       </c>
-      <c r="L226" t="inlineStr"/>
+      <c r="L226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Morgan Lee( Orlando FL,) Pending case closure </t>
+        </is>
+      </c>
       <c r="M226" t="inlineStr">
         <is>
           <t>ES &amp;PPT's</t>
@@ -12048,7 +12672,7 @@
       <c r="W226" t="inlineStr"/>
       <c r="X226" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>
@@ -12072,7 +12696,11 @@
           <t>Case Closed</t>
         </is>
       </c>
-      <c r="L227" t="inlineStr"/>
+      <c r="L227" t="inlineStr">
+        <is>
+          <t>Avery Wilson(Lake worth FL, WPB) Pending Closure</t>
+        </is>
+      </c>
       <c r="M227" t="inlineStr">
         <is>
           <t>Employment Service Only</t>
@@ -12099,7 +12727,7 @@
       <c r="W227" t="inlineStr"/>
       <c r="X227" t="inlineStr">
         <is>
-          <t>CLIENT NAME (END DATE ONLY): Missing/Invalid; CLIENT NAME (END DATE ONLY): Duplicate; Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
+          <t>Latest Check-In Date: Missing/Invalid; Latest Check-In Date: Duplicate; Latest Check-In Date.1: Missing/Invalid; Latest Check-In Date.1: Duplicate</t>
         </is>
       </c>
     </row>

</xml_diff>